<commit_message>
Writing data to csv file
</commit_message>
<xml_diff>
--- a/datasets/titanic/titanic.xlsx
+++ b/datasets/titanic/titanic.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PSP\PythonProjects\python-data-analysis\datasets\titanic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26520A4-2DC0-4185-84C3-DD4B23263956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F57DDFC-401A-4838-9E7C-EACE7B59B7B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2652" yWindow="2652" windowWidth="15120" windowHeight="8652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="titanic" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">titanic!$F$1:$F$892</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">titanic!$B$1:$B$892</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -4292,8 +4292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L892"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A867" workbookViewId="0">
-      <selection activeCell="N822" sqref="N822"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B250" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35601,7 +35601,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F892" xr:uid="{89EA898F-86CD-4CCE-A33C-2CD5F16815AF}"/>
+  <autoFilter ref="B1:B892" xr:uid="{61EBD8C4-C2D5-4432-8089-94C26D2030EE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>